<commit_message>
Initial sprint 3 document.  Updated Gantt chart for this week
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297CD2B8-6B90-7B46-9B99-8B463A4DC65C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -399,7 +394,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,12 +467,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -497,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,15 +515,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -538,6 +532,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,29 +839,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -910,13 +905,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -928,15 +923,15 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -946,61 +941,61 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="42" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:15" ht="44" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1008,16 +1003,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="J7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1027,14 +1022,14 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1043,17 +1038,17 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="42" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:15" ht="44" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1"/>
@@ -1065,12 +1060,12 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1086,9 +1081,9 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1096,46 +1091,46 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="11"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="11"/>
+      <c r="J12" s="10"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="11"/>
+      <c r="N12" s="10"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="12" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="12" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="12" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="12" t="s">
+      <c r="M13" s="12"/>
+      <c r="N13" s="11" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to reflect parallel strategy; added diagrams for presentation
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297CD2B8-6B90-7B46-9B99-8B463A4DC65C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A5BAA-515C-A341-B4E4-7C941A3E1306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,18 +440,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -508,21 +502,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -531,8 +524,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,7 +843,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N13" sqref="A1:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,9 +902,9 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -929,9 +922,9 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -942,18 +935,18 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -966,12 +959,12 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="7"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -984,12 +977,12 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1002,11 +995,11 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="J7" s="7"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1021,9 +1014,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1038,17 +1032,17 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1"/>
@@ -1060,9 +1054,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -1081,7 +1075,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="6"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1091,46 +1085,46 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="10"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="10"/>
+      <c r="N12" s="9"/>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="11" t="s">
+      <c r="I13" s="11"/>
+      <c r="J13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="11" t="s">
+      <c r="K13" s="11"/>
+      <c r="L13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="12"/>
-      <c r="N13" s="11" t="s">
+      <c r="M13" s="11"/>
+      <c r="N13" s="10" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor tweaks to PPT and stretched out dev timeline for some tasks
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A5BAA-515C-A341-B4E4-7C941A3E1306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F3ADE4-7DAB-6648-989F-40A2F02C6C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -843,7 +843,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="A1:N13"/>
+      <selection sqref="A1:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -943,7 +943,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="14"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -961,7 +961,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="14"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>

</xml_diff>

<commit_message>
Initial sprint 4 presentation deliverable added. Updates to project plan
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F3ADE4-7DAB-6648-989F-40A2F02C6C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D4F12E-BF56-A44C-BD64-D7851A73A8B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -843,7 +843,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -942,8 +942,8 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="14"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -960,8 +960,8 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
@@ -978,8 +978,8 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="7"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -996,8 +996,8 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="5"/>
       <c r="J7" s="6"/>
       <c r="K7" s="1"/>
@@ -1032,7 +1032,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1085,7 +1085,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="1"/>
       <c r="H12" s="9"/>
       <c r="I12" s="1"/>

</xml_diff>

<commit_message>
Updated schedule to reflect rolling in FHIR validation into parsers
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D4F12E-BF56-A44C-BD64-D7851A73A8B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB363308-0BB6-6047-8E2C-787509AADF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>#1</t>
   </si>
@@ -289,30 +289,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>JSON Parser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-(Developers)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FHIR Server Validation</t>
     </r>
     <r>
       <rPr>
@@ -440,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,12 +449,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -502,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -512,10 +482,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -525,7 +494,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -902,9 +871,9 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -922,8 +891,8 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
@@ -935,16 +904,16 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="6"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="1"/>
@@ -959,10 +928,10 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
       <c r="K5" s="1"/>
@@ -977,11 +946,10 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="5"/>
       <c r="J6" s="6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -995,11 +963,12 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="5"/>
-      <c r="J7" s="6"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1007,43 +976,43 @@
     </row>
     <row r="8" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
+      <c r="A9" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>32</v>
+      <c r="A10" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1054,77 +1023,59 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="5"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10" t="s">
+      <c r="I12" s="10"/>
+      <c r="J12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="10" t="s">
+      <c r="K12" s="10"/>
+      <c r="L12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="10" t="s">
+      <c r="M12" s="10"/>
+      <c r="N12" s="9" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates for project plan along with initial sprint 6 PPT
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB49CA7A-2464-394F-9AF1-6C9F4D5D52A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62284ECD-0094-7F4B-AF59-E80BB9B1BF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,9 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -983,10 +981,10 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -1001,8 +999,8 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="1"/>
@@ -1020,7 +1018,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="1"/>

</xml_diff>

<commit_message>
Team Sprint 7 updates
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62284ECD-0094-7F4B-AF59-E80BB9B1BF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F8700B-8340-D24A-AD71-2A5BDADA2BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,12 +433,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,19 +478,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -505,11 +498,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,7 +818,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -884,9 +878,9 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -904,8 +898,8 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
@@ -917,16 +911,16 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="1"/>
@@ -941,11 +935,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="6"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -959,10 +953,10 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
       <c r="J6" s="6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -980,11 +974,11 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -996,17 +990,17 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="1"/>
@@ -1018,9 +1012,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -1049,46 +1043,46 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="8"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="8"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="8"/>
+      <c r="N11" s="7"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="9" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="9" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pulled in use case model, DB mapping, moved images to images dir, and made a few cosmetic changes to Design.md
</commit_message>
<xml_diff>
--- a/collateral/Gantt Chart CS6440 Project.xlsx
+++ b/collateral/Gantt Chart CS6440 Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/school/cs6440_nfr/collateral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D8B68B-AF40-7047-8C3F-D2EACD46D0AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4341D46-9F47-C341-BB39-7170C5465454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,12 +433,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -462,11 +456,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -475,19 +478,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,7 +811,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,9 +870,9 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -884,8 +890,8 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
@@ -897,16 +903,16 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="1"/>
@@ -921,11 +927,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="5"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -939,10 +945,10 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
       <c r="J6" s="5"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -960,11 +966,11 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -976,17 +982,17 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="44" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="1"/>
@@ -998,9 +1004,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="44" x14ac:dyDescent="0.25">
@@ -1019,7 +1025,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="12"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1029,46 +1035,46 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="12"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="6" t="s">
+      <c r="K12" s="6"/>
+      <c r="L12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="6"/>
+      <c r="N12" s="13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>